<commit_message>
New Legacy Login added.
</commit_message>
<xml_diff>
--- a/Resources/Credential.xlsx
+++ b/Resources/Credential.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
   <si>
     <t xml:space="preserve">How many Quanity? </t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t>4164</t>
+  </si>
+  <si>
+    <t>Core Legacy</t>
+  </si>
+  <si>
+    <t>New Legacy</t>
+  </si>
+  <si>
+    <t>21345</t>
+  </si>
+  <si>
+    <t>4500</t>
   </si>
 </sst>
 </file>
@@ -210,15 +222,39 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -226,20 +262,113 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -527,49 +656,68 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.44140625" customWidth="1"/>
     <col min="2" max="2" width="37.109375" customWidth="1"/>
-    <col min="3" max="3" width="83" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
     <col min="4" max="4" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="17"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B2" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B3" s="7" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B4" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="13"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -579,16 +727,16 @@
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -596,7 +744,7 @@
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -604,7 +752,7 @@
       <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -612,7 +760,7 @@
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -620,7 +768,7 @@
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -628,7 +776,7 @@
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -636,7 +784,7 @@
       <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -644,7 +792,7 @@
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>28</v>
       </c>
     </row>
@@ -652,7 +800,7 @@
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -660,7 +808,7 @@
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -668,7 +816,7 @@
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -676,7 +824,7 @@
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -684,7 +832,7 @@
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -692,7 +840,7 @@
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>34</v>
       </c>
     </row>
@@ -700,7 +848,7 @@
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -708,7 +856,7 @@
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -716,7 +864,7 @@
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -724,7 +872,7 @@
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -732,7 +880,7 @@
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>39</v>
       </c>
     </row>
@@ -740,7 +888,7 @@
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>40</v>
       </c>
     </row>
@@ -748,15 +896,19 @@
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the portal creation Script, Enter data from Excel Sheet
</commit_message>
<xml_diff>
--- a/Resources/Credential.xlsx
+++ b/Resources/Credential.xlsx
@@ -19,37 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
-  <si>
-    <t>Ayso : Staging</t>
-  </si>
-  <si>
-    <t>14001</t>
-  </si>
-  <si>
-    <t>NonAyso : Staging : tshq</t>
-  </si>
-  <si>
-    <t>NonAyso : Staging : sports</t>
-  </si>
-  <si>
-    <t>4164</t>
-  </si>
-  <si>
-    <t>Core Legacy</t>
-  </si>
-  <si>
-    <t>New Legacy</t>
-  </si>
-  <si>
-    <t>4500</t>
-  </si>
-  <si>
-    <t>24904</t>
-  </si>
-  <si>
-    <t>24905</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
   <si>
     <t>Test Data to create the portals for any server</t>
   </si>
@@ -63,29 +33,59 @@
     <t>password</t>
   </si>
   <si>
-    <t>http://clubs.bluesombrero.com/Default.aspx?portalid=15</t>
-  </si>
-  <si>
-    <t>Harshid_host</t>
-  </si>
-  <si>
-    <t>Hbd@1155</t>
-  </si>
-  <si>
     <t>Portal Range</t>
   </si>
   <si>
-    <t>276</t>
-  </si>
-  <si>
     <t>278</t>
+  </si>
+  <si>
+    <t>vipul24904</t>
+  </si>
+  <si>
+    <t>vipul24905</t>
+  </si>
+  <si>
+    <t>Core Legacy Login As Admin</t>
+  </si>
+  <si>
+    <t>New Legacy Login As Admin</t>
+  </si>
+  <si>
+    <t>Login As Host</t>
+  </si>
+  <si>
+    <t>athost</t>
+  </si>
+  <si>
+    <t>ITW3546ctyz10@</t>
+  </si>
+  <si>
+    <t>St4ckSp0rts@</t>
+  </si>
+  <si>
+    <t>https://stagingtshq.bsbtest.com/Default.aspx?portalid=24904</t>
+  </si>
+  <si>
+    <t>Site Alias:</t>
+  </si>
+  <si>
+    <t>Title:</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>277</t>
+  </si>
+  <si>
+    <t>https://stagingtshq.bsbtest.com/Default.aspx?portalid=24905</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -109,8 +109,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,30 +125,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -207,15 +207,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thick">
         <color auto="1"/>
       </right>
@@ -241,52 +232,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -571,198 +553,238 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.44140625" customWidth="1"/>
-    <col min="2" max="2" width="37.109375" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53" customWidth="1"/>
+    <col min="3" max="3" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="50.6640625" customWidth="1"/>
+    <col min="5" max="5" width="45.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" ht="16.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="8"/>
+    </row>
+    <row r="7" spans="1:6" ht="27" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
+      <c r="B11" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="21"/>
-    </row>
-    <row r="7" spans="1:4" ht="27" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="18" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="19" t="s">
+      <c r="B12" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="B13" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24"/>
-      <c r="B11" s="26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
     </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="3"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="3"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="3"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://stagingtshq.bsbtest.com/Default.aspx?portalid="/>
+    <hyperlink ref="C2" r:id="rId2" display="https://stagingtshq.bsbtest.com/Default.aspx?portalid="/>
+    <hyperlink ref="E2" r:id="rId3" display="https://stagingtshq.bsbtest.com/Default.aspx?portalid="/>
+    <hyperlink ref="D2" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Program Archived Script finished
</commit_message>
<xml_diff>
--- a/Resources/Credential.xlsx
+++ b/Resources/Credential.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>Test Data to create the portals for any server</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Portal Range</t>
   </si>
   <si>
-    <t>vipul24904</t>
-  </si>
-  <si>
     <t>vipul24905</t>
   </si>
   <si>
@@ -88,6 +85,15 @@
   </si>
   <si>
     <t>315</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://testing.bsbtest.com/default.aspx?portalid=1369 </t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>fnw00t#</t>
   </si>
 </sst>
 </file>
@@ -565,7 +571,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -580,15 +586,15 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="19"/>
       <c r="E1" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="19"/>
     </row>
@@ -597,19 +603,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -617,19 +623,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -637,19 +643,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -666,7 +672,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -674,7 +680,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -682,7 +688,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -690,29 +696,29 @@
         <v>4</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>15</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New Reg Program Creation Step 1 Program Setting
</commit_message>
<xml_diff>
--- a/Resources/Credential.xlsx
+++ b/Resources/Credential.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Test Data to create the portals for any server</t>
   </si>
@@ -72,28 +72,16 @@
     <t>https://stagingtshq.bsbtest.com/Default.aspx?portalid=24905</t>
   </si>
   <si>
-    <t>https://clubs.bluesombrero.com/Default.aspx?portalid=15</t>
-  </si>
-  <si>
-    <t>Harshid_host</t>
-  </si>
-  <si>
-    <t>Hbd@1155</t>
-  </si>
-  <si>
-    <t>215</t>
-  </si>
-  <si>
-    <t>315</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://testing.bsbtest.com/default.aspx?portalid=1369 </t>
-  </si>
-  <si>
-    <t>host</t>
-  </si>
-  <si>
-    <t>fnw00t#</t>
+    <t xml:space="preserve">http://testing.bsbtest.com/default.aspx?portalid=1141 </t>
+  </si>
+  <si>
+    <t>bsbadmin1141</t>
+  </si>
+  <si>
+    <t>Old4thWard#</t>
+  </si>
+  <si>
+    <t>2152</t>
   </si>
 </sst>
 </file>
@@ -571,7 +559,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -603,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>1</v>
@@ -623,7 +611,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
@@ -643,7 +631,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>3</v>
@@ -672,7 +660,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -680,7 +668,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -688,7 +676,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -702,7 +690,7 @@
     <row r="11" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="17"/>
       <c r="B11" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
properties file added for the file path
</commit_message>
<xml_diff>
--- a/Resources/Credential.xlsx
+++ b/Resources/Credential.xlsx
@@ -305,23 +305,23 @@
     <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -609,7 +609,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:B14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -623,18 +623,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="19"/>
-      <c r="E1" s="18" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="19"/>
+      <c r="F1" s="22"/>
     </row>
     <row r="2" spans="1:6" ht="16.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -700,10 +700,10 @@
       <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="19"/>
+      <c r="B6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -730,7 +730,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="9" t="s">
@@ -738,7 +738,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="10" t="s">
         <v>24</v>
       </c>
@@ -760,96 +760,96 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="19"/>
+      <c r="B14" s="22"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="19" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="19" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="23" t="s">
+      <c r="B18" s="19" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="18" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="19" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="19" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="19" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="19" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="20" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
vipul commit after  VPPersonalPC branch merge
</commit_message>
<xml_diff>
--- a/Resources/Credential.xlsx
+++ b/Resources/Credential.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -90,12 +91,6 @@
     <t>H@rshid@1155</t>
   </si>
   <si>
-    <t>35</t>
-  </si>
-  <si>
-    <t>334</t>
-  </si>
-  <si>
     <t>https://tshq.bluesombrero.com/Default.aspx?portalid=20001</t>
   </si>
   <si>
@@ -127,6 +122,12 @@
   </si>
   <si>
     <t>Bulk Mail Urls and Credintials</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>111</t>
   </si>
 </sst>
 </file>
@@ -609,7 +610,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -734,13 +735,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24"/>
       <c r="B11" s="10" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -761,7 +762,7 @@
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14" s="22"/>
     </row>
@@ -770,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -778,7 +779,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -786,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -794,7 +795,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -802,7 +803,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -810,7 +811,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -818,7 +819,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -826,7 +827,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -834,7 +835,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -842,7 +843,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Vipul, after Hiral Changed Merged.
</commit_message>
<xml_diff>
--- a/Resources/Credential.xlsx
+++ b/Resources/Credential.xlsx
@@ -15,12 +15,11 @@
     <sheet name="Credentials" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>Test Data to create the portals for any server</t>
   </si>
@@ -73,15 +72,6 @@
     <t>https://stagingtshq.bsbtest.com/Default.aspx?portalid=24905</t>
   </si>
   <si>
-    <t xml:space="preserve">http://testing.bsbtest.com/default.aspx?portalid=1141 </t>
-  </si>
-  <si>
-    <t>bsbadmin1141</t>
-  </si>
-  <si>
-    <t>Old4thWard#</t>
-  </si>
-  <si>
     <t>https://clubs.bluesombrero.com/Default.aspx?portalid=15</t>
   </si>
   <si>
@@ -128,6 +118,12 @@
   </si>
   <si>
     <t>111</t>
+  </si>
+  <si>
+    <t>#Sp0rtsC0nn3ct</t>
+  </si>
+  <si>
+    <t>vipul24904</t>
   </si>
 </sst>
 </file>
@@ -610,7 +606,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -641,8 +637,8 @@
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>17</v>
+      <c r="B2" s="19" t="s">
+        <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>1</v>
@@ -661,8 +657,8 @@
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>18</v>
+      <c r="B3" s="19" t="s">
+        <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
@@ -681,8 +677,8 @@
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>19</v>
+      <c r="B4" s="20" t="s">
+        <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>3</v>
@@ -711,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -719,7 +715,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -727,7 +723,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -735,13 +731,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24"/>
       <c r="B11" s="10" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -762,7 +758,7 @@
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B14" s="22"/>
     </row>
@@ -771,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -779,7 +775,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -787,7 +783,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -795,7 +791,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -803,7 +799,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -811,7 +807,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -819,7 +815,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -827,7 +823,7 @@
         <v>2</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -835,7 +831,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -843,7 +839,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -851,7 +847,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Vipul after date function change for the year 2021
</commit_message>
<xml_diff>
--- a/Resources/Credential.xlsx
+++ b/Resources/Credential.xlsx
@@ -114,16 +114,16 @@
     <t>Bulk Mail Urls and Credintials</t>
   </si>
   <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
     <t>#Sp0rtsC0nn3ct</t>
   </si>
   <si>
     <t>vipul24904</t>
+  </si>
+  <si>
+    <t>426</t>
+  </si>
+  <si>
+    <t>500</t>
   </si>
 </sst>
 </file>
@@ -658,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>2</v>
@@ -731,13 +731,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="24"/>
       <c r="B11" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -847,7 +847,7 @@
         <v>3</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">

</xml_diff>